<commit_message>
Add n/a to resp 2
</commit_message>
<xml_diff>
--- a/cognitive task model/002-cognitive task.xlsx
+++ b/cognitive task model/002-cognitive task.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
   <si>
     <t>Time Started</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Supporting Material</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Focus</t>
   </si>
   <si>
@@ -73,7 +70,7 @@
     <t>Conclude</t>
   </si>
   <si>
-    <t>End</t>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -98,7 +95,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -130,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="21" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -144,11 +141,8 @@
     <xf xfId="0" numFmtId="21" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="21" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -461,16 +455,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="17.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="17.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="7" width="18.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="18.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="6" width="18.433571428571426" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -491,9 +485,9 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="4">
-        <v>0.9997916666666666</v>
+        <v>1.9993287037037037</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -507,57 +501,47 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="4">
+        <v>2.000636574074074</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="4">
-        <v>1.001099537037037</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="J3" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4">
-        <v>1.0013541666666668</v>
+        <v>2.000891203703704</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="J4" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="4">
-        <v>1.0016319444444444</v>
+        <v>2.0011689814814817</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>3</v>
@@ -567,91 +551,75 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-      <c r="J5" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="J5" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4">
-        <v>1.0017592592592592</v>
+        <v>2.0012962962962964</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="J6" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4">
-        <v>1.0017824074074073</v>
+        <v>2.0013194444444444</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="J7" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="4">
-        <v>1.0028935185185186</v>
+        <v>2.0024305555555557</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="J8" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="4">
-        <v>1.0029976851851852</v>
+        <v>2.0025347222222223</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -659,13 +627,11 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="J9" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="4">
-        <v>1.0035416666666668</v>
+        <v>2.0030787037037037</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>3</v>
@@ -679,19 +645,17 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="J10" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="4">
-        <v>1.0037615740740742</v>
+        <v>2.003298611111111</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -699,19 +663,17 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="J11" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="4">
-        <v>1.0039120370370371</v>
+        <v>2.003449074074074</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -719,16 +681,14 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="J12" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4">
-        <v>1.0044097222222221</v>
+        <v>2.003946759259259</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>4</v>
@@ -743,13 +703,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="4">
-        <v>1.004513888888889</v>
+        <v>2.0040509259259256</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -761,13 +721,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="4">
-        <v>1.004675925925926</v>
+        <v>2.004212962962963</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -779,13 +739,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="4">
-        <v>1.0049768518518518</v>
+        <v>2.004513888888889</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -797,10 +757,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="4">
-        <v>1.0054976851851851</v>
+        <v>2.0050347222222222</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -813,13 +773,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="4">
-        <v>1.0055555555555555</v>
+        <v>2.0050925925925926</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -831,10 +791,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="4">
-        <v>1.0063425925925926</v>
+        <v>2.0058796296296295</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>

</xml_diff>